<commit_message>
updated worksheet to include cfm majors. fixed typo on instructions.
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-Class-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-Class-Lookups-Match-IF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A73A05-9D89-984E-A7D0-DDD440D490CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE782D3-B217-4747-99AD-78C223B262FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31440" yWindow="3220" windowWidth="34060" windowHeight="20820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35240" yWindow="3320" windowWidth="31820" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="Employee Work Hours" sheetId="5" r:id="rId3"/>
     <sheet name="Concrete Price Estimator" sheetId="3" r:id="rId4"/>
     <sheet name="School Left" sheetId="6" r:id="rId5"/>
-    <sheet name="School Dropdown" sheetId="7" state="hidden" r:id="rId6"/>
+    <sheet name="School Dropdown" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="5" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="126">
   <si>
     <t>MATERIAL COST &amp; AVAILABILITY</t>
   </si>
@@ -355,12 +355,6 @@
     <t>What is your year?</t>
   </si>
   <si>
-    <t>If not Engineering, then Years = 0</t>
-  </si>
-  <si>
-    <t>If any Engineering, then Years = 1</t>
-  </si>
-  <si>
     <t>What is your major?</t>
   </si>
   <si>
@@ -397,9 +391,6 @@
     <t>Freshman</t>
   </si>
   <si>
-    <t>I'm not an Engineer :(</t>
-  </si>
-  <si>
     <t>Electrical Engineering</t>
   </si>
   <si>
@@ -413,6 +404,21 @@
   </si>
   <si>
     <t>Civil Engineering</t>
+  </si>
+  <si>
+    <t>Construction Management</t>
+  </si>
+  <si>
+    <t>Facility and Property Management</t>
+  </si>
+  <si>
+    <t>Other :(</t>
+  </si>
+  <si>
+    <t>If any Engineering/CFM, then Years = 1</t>
+  </si>
+  <si>
+    <t>If not Engineering/CFM, then Years = 0</t>
   </si>
 </sst>
 </file>
@@ -942,6 +948,58 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="6" xfId="2" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="5" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -951,6 +1009,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
@@ -970,70 +1040,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="13" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="15" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="14" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="15" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1648,7 +1654,7 @@
   <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1658,160 +1664,160 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="50" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
+      <c r="A2" s="51"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
     </row>
     <row r="3" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="35"/>
-      <c r="C3" s="62" t="s">
+      <c r="B3" s="53"/>
+      <c r="C3" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="47" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A4" s="59" t="s">
+      <c r="A4" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="60" t="s">
+      <c r="B4" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="64">
+      <c r="C4" s="49">
         <v>130</v>
       </c>
-      <c r="D4" s="63">
+      <c r="D4" s="48">
         <v>416</v>
       </c>
       <c r="F4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="44" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="64">
+      <c r="C5" s="49">
         <v>900</v>
       </c>
-      <c r="D5" s="63">
+      <c r="D5" s="48">
         <v>462</v>
       </c>
       <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="61" t="s">
+      <c r="B6" s="46" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="64">
+      <c r="C6" s="49">
         <v>125</v>
       </c>
-      <c r="D6" s="63">
+      <c r="D6" s="48">
         <v>178</v>
       </c>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A7" s="59" t="s">
+      <c r="A7" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="61" t="s">
+      <c r="B7" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="64">
+      <c r="C7" s="49">
         <v>5</v>
       </c>
-      <c r="D7" s="63">
+      <c r="D7" s="48">
         <v>200</v>
       </c>
       <c r="F7" s="1"/>
     </row>
     <row r="8" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A8" s="59" t="s">
+      <c r="A8" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="61" t="s">
+      <c r="B8" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="64">
+      <c r="C8" s="49">
         <v>40</v>
       </c>
-      <c r="D8" s="63">
+      <c r="D8" s="48">
         <v>190</v>
       </c>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A9" s="59" t="s">
+      <c r="A9" s="44" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="64">
+      <c r="B9" s="46"/>
+      <c r="C9" s="49">
         <v>0.67</v>
       </c>
-      <c r="D9" s="63">
+      <c r="D9" s="48">
         <v>321</v>
       </c>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A10" s="59" t="s">
+      <c r="A10" s="44" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="61" t="s">
+      <c r="B10" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="64">
+      <c r="C10" s="49">
         <v>2500</v>
       </c>
-      <c r="D10" s="63">
+      <c r="D10" s="48">
         <v>112</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A11" s="59" t="s">
+      <c r="A11" s="44" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="61" t="s">
+      <c r="B11" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="64">
+      <c r="C11" s="49">
         <v>50</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="48">
         <v>383</v>
       </c>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:6" ht="13" x14ac:dyDescent="0.15">
-      <c r="A12" s="59" t="s">
+      <c r="A12" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="61" t="s">
+      <c r="B12" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="64">
+      <c r="C12" s="49">
         <v>150</v>
       </c>
-      <c r="D12" s="63">
+      <c r="D12" s="48">
         <v>356</v>
       </c>
       <c r="F12" s="1"/>
@@ -1920,20 +1926,20 @@
       <c r="B2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="57">
+      <c r="C2" s="42">
         <v>98</v>
       </c>
-      <c r="D2" s="52"/>
-      <c r="E2" s="53"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="38"/>
       <c r="G2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="34">
         <f t="shared" ref="H2:H10" si="0">SUMIF($B$2:$B$30,G2,$C$2:$C$30)</f>
         <v>238</v>
       </c>
-      <c r="I2" s="51"/>
-      <c r="J2" s="56"/>
+      <c r="I2" s="36"/>
+      <c r="J2" s="41"/>
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
@@ -1942,20 +1948,20 @@
       <c r="B3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="57">
+      <c r="C3" s="42">
         <v>76</v>
       </c>
-      <c r="D3" s="52"/>
-      <c r="E3" s="53"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38"/>
       <c r="G3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="49">
+      <c r="H3" s="34">
         <f t="shared" si="0"/>
         <v>336</v>
       </c>
-      <c r="I3" s="51"/>
-      <c r="J3" s="56"/>
+      <c r="I3" s="36"/>
+      <c r="J3" s="41"/>
     </row>
     <row r="4" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="4" t="s">
@@ -1964,21 +1970,21 @@
       <c r="B4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="57">
+      <c r="C4" s="42">
         <v>87</v>
       </c>
-      <c r="D4" s="52"/>
-      <c r="E4" s="53"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="6"/>
       <c r="G4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H4" s="49">
+      <c r="H4" s="34">
         <f t="shared" si="0"/>
         <v>216</v>
       </c>
-      <c r="I4" s="51"/>
-      <c r="J4" s="56"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
@@ -1987,21 +1993,21 @@
       <c r="B5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="57">
+      <c r="C5" s="42">
         <v>81</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="E5" s="53"/>
+      <c r="D5" s="37"/>
+      <c r="E5" s="38"/>
       <c r="F5" s="6"/>
       <c r="G5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="49">
+      <c r="H5" s="34">
         <f t="shared" si="0"/>
         <v>324</v>
       </c>
-      <c r="I5" s="51"/>
-      <c r="J5" s="56"/>
+      <c r="I5" s="36"/>
+      <c r="J5" s="41"/>
     </row>
     <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="4" t="s">
@@ -2010,21 +2016,21 @@
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="57">
+      <c r="C6" s="42">
         <v>84</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="53"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="38"/>
       <c r="F6" s="6"/>
       <c r="G6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="34">
         <f t="shared" si="0"/>
         <v>239</v>
       </c>
-      <c r="I6" s="51"/>
-      <c r="J6" s="56"/>
+      <c r="I6" s="36"/>
+      <c r="J6" s="41"/>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="4" t="s">
@@ -2033,21 +2039,21 @@
       <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="57">
+      <c r="C7" s="42">
         <v>2500</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="53"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38"/>
       <c r="F7" s="6"/>
       <c r="G7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="34">
         <f t="shared" si="0"/>
         <v>9750</v>
       </c>
-      <c r="I7" s="51"/>
-      <c r="J7" s="56"/>
+      <c r="I7" s="36"/>
+      <c r="J7" s="41"/>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="4" t="s">
@@ -2056,21 +2062,21 @@
       <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="57">
+      <c r="C8" s="42">
         <v>90</v>
       </c>
-      <c r="D8" s="52"/>
-      <c r="E8" s="53"/>
+      <c r="D8" s="37"/>
+      <c r="E8" s="38"/>
       <c r="F8" s="6"/>
       <c r="G8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="49">
+      <c r="H8" s="34">
         <f t="shared" si="0"/>
         <v>212</v>
       </c>
-      <c r="I8" s="51"/>
-      <c r="J8" s="56"/>
+      <c r="I8" s="36"/>
+      <c r="J8" s="41"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="4" t="s">
@@ -2079,21 +2085,21 @@
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="57">
+      <c r="C9" s="42">
         <v>74</v>
       </c>
-      <c r="D9" s="52"/>
-      <c r="E9" s="53"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
       <c r="F9" s="6"/>
       <c r="G9" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="34">
         <f t="shared" si="0"/>
         <v>175</v>
       </c>
-      <c r="I9" s="51"/>
-      <c r="J9" s="56"/>
+      <c r="I9" s="36"/>
+      <c r="J9" s="41"/>
     </row>
     <row r="10" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
@@ -2102,21 +2108,21 @@
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="57">
+      <c r="C10" s="42">
         <v>56</v>
       </c>
-      <c r="D10" s="52"/>
-      <c r="E10" s="53"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="38"/>
       <c r="F10" s="6"/>
       <c r="G10" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="50">
+      <c r="H10" s="35">
         <f t="shared" si="0"/>
         <v>170</v>
       </c>
-      <c r="I10" s="54"/>
-      <c r="J10" s="47"/>
+      <c r="I10" s="39"/>
+      <c r="J10" s="32"/>
     </row>
     <row r="11" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="4" t="s">
@@ -2125,11 +2131,11 @@
       <c r="B11" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="57">
+      <c r="C11" s="42">
         <v>86</v>
       </c>
-      <c r="D11" s="52"/>
-      <c r="E11" s="53"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
       <c r="F11" s="6"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2143,11 +2149,11 @@
       <c r="B12" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="57">
+      <c r="C12" s="42">
         <v>81</v>
       </c>
-      <c r="D12" s="52"/>
-      <c r="E12" s="53"/>
+      <c r="D12" s="37"/>
+      <c r="E12" s="38"/>
       <c r="F12" s="6"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2161,11 +2167,11 @@
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="57">
+      <c r="C13" s="42">
         <v>59</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="53"/>
+      <c r="D13" s="37"/>
+      <c r="E13" s="38"/>
       <c r="F13" s="6"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2179,11 +2185,11 @@
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="57">
+      <c r="C14" s="42">
         <v>73</v>
       </c>
-      <c r="D14" s="52"/>
-      <c r="E14" s="53"/>
+      <c r="D14" s="37"/>
+      <c r="E14" s="38"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -2196,11 +2202,11 @@
       <c r="B15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="57">
+      <c r="C15" s="42">
         <v>60</v>
       </c>
-      <c r="D15" s="52"/>
-      <c r="E15" s="53"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="38"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -2213,11 +2219,11 @@
       <c r="B16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="57">
+      <c r="C16" s="42">
         <v>90</v>
       </c>
-      <c r="D16" s="52"/>
-      <c r="E16" s="53"/>
+      <c r="D16" s="37"/>
+      <c r="E16" s="38"/>
       <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
@@ -2230,11 +2236,11 @@
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="57">
+      <c r="C17" s="42">
         <v>51</v>
       </c>
-      <c r="D17" s="52"/>
-      <c r="E17" s="53"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38"/>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
@@ -2247,11 +2253,11 @@
       <c r="B18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="57">
+      <c r="C18" s="42">
         <v>64</v>
       </c>
-      <c r="D18" s="52"/>
-      <c r="E18" s="53"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
       <c r="I18" s="3"/>
@@ -2264,11 +2270,11 @@
       <c r="B19" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="57">
+      <c r="C19" s="42">
         <v>92</v>
       </c>
-      <c r="D19" s="52"/>
-      <c r="E19" s="53"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -2281,11 +2287,11 @@
       <c r="B20" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="57">
+      <c r="C20" s="42">
         <v>80</v>
       </c>
-      <c r="D20" s="52"/>
-      <c r="E20" s="53"/>
+      <c r="D20" s="37"/>
+      <c r="E20" s="38"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -2298,11 +2304,11 @@
       <c r="B21" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="57">
+      <c r="C21" s="42">
         <v>88</v>
       </c>
-      <c r="D21" s="52"/>
-      <c r="E21" s="53"/>
+      <c r="D21" s="37"/>
+      <c r="E21" s="38"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -2315,11 +2321,11 @@
       <c r="B22" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="57">
+      <c r="C22" s="42">
         <v>70</v>
       </c>
-      <c r="D22" s="52"/>
-      <c r="E22" s="53"/>
+      <c r="D22" s="37"/>
+      <c r="E22" s="38"/>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -2332,11 +2338,11 @@
       <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="57">
+      <c r="C23" s="42">
         <v>4000</v>
       </c>
-      <c r="D23" s="52"/>
-      <c r="E23" s="53"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="38"/>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
       <c r="I23" s="3"/>
@@ -2349,11 +2355,11 @@
       <c r="B24" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C24" s="57">
+      <c r="C24" s="42">
         <v>71</v>
       </c>
-      <c r="D24" s="52"/>
-      <c r="E24" s="53"/>
+      <c r="D24" s="37"/>
+      <c r="E24" s="38"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
@@ -2366,11 +2372,11 @@
       <c r="B25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="57">
+      <c r="C25" s="42">
         <v>3250</v>
       </c>
-      <c r="D25" s="52"/>
-      <c r="E25" s="53"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -2383,11 +2389,11 @@
       <c r="B26" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C26" s="57">
+      <c r="C26" s="42">
         <v>82</v>
       </c>
-      <c r="D26" s="52"/>
-      <c r="E26" s="53"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="38"/>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -2400,11 +2406,11 @@
       <c r="B27" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="57">
+      <c r="C27" s="42">
         <v>67</v>
       </c>
-      <c r="D27" s="52"/>
-      <c r="E27" s="53"/>
+      <c r="D27" s="37"/>
+      <c r="E27" s="38"/>
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -2417,11 +2423,11 @@
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="57">
+      <c r="C28" s="42">
         <v>85</v>
       </c>
-      <c r="D28" s="52"/>
-      <c r="E28" s="53"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="38"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -2434,11 +2440,11 @@
       <c r="B29" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C29" s="57">
+      <c r="C29" s="42">
         <v>64</v>
       </c>
-      <c r="D29" s="52"/>
-      <c r="E29" s="53"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="38"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -2451,11 +2457,11 @@
       <c r="B30" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C30" s="58">
+      <c r="C30" s="43">
         <v>82</v>
       </c>
-      <c r="D30" s="55"/>
-      <c r="E30" s="48"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="33"/>
       <c r="G30" s="3"/>
       <c r="H30" s="3"/>
       <c r="I30" s="3"/>
@@ -13149,7 +13155,7 @@
   <dimension ref="A1:H987"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13180,15 +13186,15 @@
     </row>
     <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="3"/>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
     </row>
     <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="24" t="s">
@@ -22350,7 +22356,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -23467,7 +23473,7 @@
   <dimension ref="B7:O23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="J13" sqref="J13:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -23492,68 +23498,68 @@
     </row>
     <row r="8" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="I8" s="28" t="s">
-        <v>111</v>
-      </c>
-      <c r="J8" s="46" t="s">
-        <v>110</v>
-      </c>
-      <c r="K8" s="46"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="46"/>
-      <c r="N8" s="46"/>
-      <c r="O8" s="46"/>
+        <v>109</v>
+      </c>
+      <c r="J8" s="58" t="s">
+        <v>108</v>
+      </c>
+      <c r="K8" s="58"/>
+      <c r="L8" s="58"/>
+      <c r="M8" s="58"/>
+      <c r="N8" s="58"/>
+      <c r="O8" s="58"/>
     </row>
     <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="26" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C9" s="30"/>
       <c r="I9" s="29"/>
-      <c r="J9" s="37" t="s">
-        <v>108</v>
-      </c>
-      <c r="K9" s="38"/>
-      <c r="L9" s="38"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="38"/>
-      <c r="O9" s="39"/>
+      <c r="J9" s="59" t="s">
+        <v>106</v>
+      </c>
+      <c r="K9" s="60"/>
+      <c r="L9" s="60"/>
+      <c r="M9" s="60"/>
+      <c r="N9" s="60"/>
+      <c r="O9" s="61"/>
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="J10" s="40" t="s">
-        <v>107</v>
-      </c>
-      <c r="K10" s="41"/>
-      <c r="L10" s="41"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="41"/>
-      <c r="O10" s="42"/>
+      <c r="J10" s="62" t="s">
+        <v>105</v>
+      </c>
+      <c r="K10" s="63"/>
+      <c r="L10" s="63"/>
+      <c r="M10" s="63"/>
+      <c r="N10" s="63"/>
+      <c r="O10" s="64"/>
     </row>
     <row r="11" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="26" t="s">
-        <v>106</v>
-      </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
+        <v>104</v>
+      </c>
+      <c r="C11" s="55"/>
+      <c r="D11" s="56"/>
+      <c r="E11" s="57"/>
       <c r="I11" s="29"/>
-      <c r="J11" s="37" t="s">
-        <v>105</v>
-      </c>
-      <c r="K11" s="38"/>
-      <c r="L11" s="38"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="38"/>
-      <c r="O11" s="39"/>
+      <c r="J11" s="59" t="s">
+        <v>124</v>
+      </c>
+      <c r="K11" s="60"/>
+      <c r="L11" s="60"/>
+      <c r="M11" s="60"/>
+      <c r="N11" s="60"/>
+      <c r="O11" s="61"/>
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="J12" s="40" t="s">
-        <v>104</v>
-      </c>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="42"/>
+      <c r="J12" s="62" t="s">
+        <v>125</v>
+      </c>
+      <c r="K12" s="63"/>
+      <c r="L12" s="63"/>
+      <c r="M12" s="63"/>
+      <c r="N12" s="63"/>
+      <c r="O12" s="64"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B13" s="26" t="s">
@@ -23561,24 +23567,24 @@
       </c>
       <c r="C13" s="30"/>
       <c r="I13" s="27"/>
-      <c r="J13" s="37" t="s">
+      <c r="J13" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="K13" s="38"/>
-      <c r="L13" s="38"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="38"/>
-      <c r="O13" s="39"/>
+      <c r="K13" s="60"/>
+      <c r="L13" s="60"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="60"/>
+      <c r="O13" s="61"/>
     </row>
     <row r="14" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="J14" s="40" t="s">
+      <c r="J14" s="62" t="s">
         <v>101</v>
       </c>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="42"/>
+      <c r="K14" s="63"/>
+      <c r="L14" s="63"/>
+      <c r="M14" s="63"/>
+      <c r="N14" s="63"/>
+      <c r="O14" s="64"/>
     </row>
     <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="26" t="s">
@@ -23586,24 +23592,24 @@
       </c>
       <c r="C15" s="30"/>
       <c r="I15" s="27"/>
-      <c r="J15" s="37" t="s">
+      <c r="J15" s="59" t="s">
         <v>99</v>
       </c>
-      <c r="K15" s="38"/>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="38"/>
-      <c r="O15" s="39"/>
+      <c r="K15" s="60"/>
+      <c r="L15" s="60"/>
+      <c r="M15" s="60"/>
+      <c r="N15" s="60"/>
+      <c r="O15" s="61"/>
     </row>
     <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="J16" s="40" t="s">
+      <c r="J16" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="K16" s="41"/>
-      <c r="L16" s="41"/>
-      <c r="M16" s="41"/>
-      <c r="N16" s="41"/>
-      <c r="O16" s="42"/>
+      <c r="K16" s="63"/>
+      <c r="L16" s="63"/>
+      <c r="M16" s="63"/>
+      <c r="N16" s="63"/>
+      <c r="O16" s="64"/>
     </row>
     <row r="17" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="26" t="s">
@@ -23611,24 +23617,24 @@
       </c>
       <c r="F17" s="30"/>
       <c r="I17" s="27"/>
-      <c r="J17" s="37" t="s">
+      <c r="J17" s="59" t="s">
         <v>97</v>
       </c>
-      <c r="K17" s="38"/>
-      <c r="L17" s="38"/>
-      <c r="M17" s="38"/>
-      <c r="N17" s="38"/>
-      <c r="O17" s="39"/>
+      <c r="K17" s="60"/>
+      <c r="L17" s="60"/>
+      <c r="M17" s="60"/>
+      <c r="N17" s="60"/>
+      <c r="O17" s="61"/>
     </row>
     <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="J18" s="40" t="s">
+      <c r="J18" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="K18" s="41"/>
-      <c r="L18" s="41"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="41"/>
-      <c r="O18" s="42"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="63"/>
+      <c r="M18" s="63"/>
+      <c r="N18" s="63"/>
+      <c r="O18" s="64"/>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
@@ -23636,24 +23642,24 @@
       </c>
       <c r="C19" s="30"/>
       <c r="I19" s="29"/>
-      <c r="J19" s="37" t="s">
+      <c r="J19" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="K19" s="38"/>
-      <c r="L19" s="38"/>
-      <c r="M19" s="38"/>
-      <c r="N19" s="38"/>
-      <c r="O19" s="39"/>
+      <c r="K19" s="60"/>
+      <c r="L19" s="60"/>
+      <c r="M19" s="60"/>
+      <c r="N19" s="60"/>
+      <c r="O19" s="61"/>
     </row>
     <row r="20" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="J20" s="40" t="s">
+      <c r="J20" s="62" t="s">
         <v>93</v>
       </c>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="42"/>
+      <c r="K20" s="63"/>
+      <c r="L20" s="63"/>
+      <c r="M20" s="63"/>
+      <c r="N20" s="63"/>
+      <c r="O20" s="64"/>
     </row>
     <row r="22" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="I22" s="28" t="s">
@@ -23668,6 +23674,7 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="C11:E11"/>
     <mergeCell ref="J8:O8"/>
     <mergeCell ref="J17:O17"/>
     <mergeCell ref="J18:O18"/>
@@ -23681,7 +23688,6 @@
     <mergeCell ref="J14:O14"/>
     <mergeCell ref="J15:O15"/>
     <mergeCell ref="J16:O16"/>
-    <mergeCell ref="C11:E11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -23697,19 +23703,19 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E20CAD0E-ECD3-481A-B04D-FAFB4CEDB953}">
           <x14:formula1>
-            <xm:f>'School Dropdown'!$A$4:$A$9</xm:f>
+            <xm:f>'School Dropdown'!$A$4:$A$11</xm:f>
           </x14:formula1>
           <xm:sqref>C11:E11</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9C6A3ECB-0881-4F12-A425-76C41BF68F2A}">
           <x14:formula1>
-            <xm:f>'School Dropdown'!$A$11:$A$14</xm:f>
+            <xm:f>'School Dropdown'!$A$13:$A$16</xm:f>
           </x14:formula1>
           <xm:sqref>C13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1C7D121F-E5FF-4E03-B67D-6192D28B0202}">
           <x14:formula1>
-            <xm:f>'School Dropdown'!$A$17:$A$34</xm:f>
+            <xm:f>'School Dropdown'!$A$19:$A$36</xm:f>
           </x14:formula1>
           <xm:sqref>F17</xm:sqref>
         </x14:dataValidation>
@@ -23722,10 +23728,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28BE5E5-B39C-4AB3-96A9-546FFB6E312D}">
   <sheetPr codeName="Sheet2"/>
-  <dimension ref="A1:A34"/>
+  <dimension ref="A1:A36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L44" sqref="L44"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -23735,52 +23741,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A1" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A2" s="26" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A4" s="26" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A5" s="26" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A6" s="26" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A7" s="26" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A8" s="26" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A9" s="26" t="s">
-        <v>118</v>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A10" s="26" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A11" s="26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="26" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
@@ -23793,93 +23799,103 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A17" s="26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A18" s="26">
-        <v>2</v>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" s="26" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" s="26" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A19" s="26">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A20" s="26">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A21" s="26">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A22" s="26">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A23" s="26">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A24" s="26">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A25" s="26">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A26" s="26">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A27" s="26">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A28" s="26">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A29" s="26">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A30" s="26">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A31" s="26">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A32" s="26">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A33" s="26">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.15">
       <c r="A34" s="26">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A35" s="26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A36" s="26">
         <v>18</v>
       </c>
     </row>

</xml_diff>

<commit_message>
removed data validation from in-class workbook (we do that in next unit)
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-Class-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-Class-Lookups-Match-IF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DE782D3-B217-4747-99AD-78C223B262FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FF84509-5811-DC4C-890C-B8E0B72CFEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35240" yWindow="3320" windowWidth="31820" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35240" yWindow="3320" windowWidth="31820" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Materials" sheetId="1" r:id="rId1"/>
@@ -1653,8 +1653,8 @@
   </sheetPr>
   <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1876,8 +1876,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -13144,6 +13144,18 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{65A1DE97-3F39-CD4E-B25E-1262F9D91CC8}">
+          <x14:formula1>
+            <xm:f>Materials!$A$4:$A$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:B30</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 

</xml_diff>